<commit_message>
Se agrego la opción para hacer comentarios sobre las tarjetas
</commit_message>
<xml_diff>
--- a/backend/PlantillasExcel/TarjetaResponsabilidad.xlsx
+++ b/backend/PlantillasExcel/TarjetaResponsabilidad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\Desktop\EPS\backend\PlantillasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9695C96-EEEC-4307-BD71-9937BCCE503B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A4CBEF-7D6E-4C74-9458-58AC8CA32F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B3EC3C9A-185F-4CCB-96F6-D3C245115DC3}"/>
   </bookViews>
@@ -794,13 +794,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,12 +1142,12 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="1" customWidth="1"/>
@@ -1156,23 +1156,23 @@
     <col min="7" max="7" width="3.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="34.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="9" customWidth="1"/>
     <col min="11" max="16384" width="8.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1203,28 +1203,28 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="5"/>
@@ -1233,7 +1233,7 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="5"/>
@@ -1242,7 +1242,7 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="5"/>
@@ -1251,7 +1251,7 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
@@ -1260,7 +1260,7 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -1269,7 +1269,7 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
@@ -1278,7 +1278,7 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
@@ -1287,7 +1287,7 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="9"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
@@ -1296,7 +1296,7 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="9"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
@@ -1305,7 +1305,7 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
@@ -1314,7 +1314,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
@@ -1323,7 +1323,7 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="9"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
@@ -1332,7 +1332,7 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
@@ -1341,7 +1341,7 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
@@ -1350,7 +1350,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
@@ -1359,7 +1359,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
+      <c r="A21" s="9"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
@@ -1368,7 +1368,7 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
@@ -1377,7 +1377,7 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
+      <c r="A23" s="9"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
@@ -1386,7 +1386,7 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
+      <c r="A24" s="9"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
@@ -1395,7 +1395,7 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
+      <c r="A25" s="9"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
@@ -1404,7 +1404,7 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="9"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
@@ -1413,7 +1413,7 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
@@ -1422,7 +1422,7 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+      <c r="A28" s="9"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
@@ -1431,7 +1431,7 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
+      <c r="A29" s="9"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
@@ -1440,7 +1440,7 @@
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
+      <c r="A30" s="9"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -1449,7 +1449,7 @@
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
+      <c r="A31" s="9"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
@@ -1458,7 +1458,7 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
@@ -1467,7 +1467,7 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+      <c r="A33" s="9"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
@@ -1476,7 +1476,7 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+      <c r="A34" s="9"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
@@ -1485,7 +1485,7 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
@@ -1494,7 +1494,7 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="A36" s="9"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
@@ -1503,7 +1503,7 @@
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="A37" s="9"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="5"/>
@@ -1512,7 +1512,7 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="A38" s="9"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
@@ -1521,7 +1521,7 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
@@ -1530,7 +1530,7 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="5"/>
@@ -1540,14 +1540,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:J1048576"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="A1:A40"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
@@ -1564,22 +1572,14 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:J1048576"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1609,23 +1609,23 @@
     <col min="7" max="7" width="3.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="34.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="9" customWidth="1"/>
     <col min="11" max="16384" width="8.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="70.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1656,28 +1656,28 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="5"/>
@@ -1686,7 +1686,7 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="5"/>
@@ -1695,7 +1695,7 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="5"/>
@@ -1704,7 +1704,7 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
@@ -1713,7 +1713,7 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -1722,7 +1722,7 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
@@ -1731,7 +1731,7 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
@@ -1740,7 +1740,7 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="9"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
@@ -1749,7 +1749,7 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="9"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
@@ -1758,7 +1758,7 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
@@ -1767,7 +1767,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
@@ -1776,7 +1776,7 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="9"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
@@ -1785,7 +1785,7 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
@@ -1794,7 +1794,7 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
@@ -1803,7 +1803,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
@@ -1812,7 +1812,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
+      <c r="A21" s="9"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
@@ -1821,7 +1821,7 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
@@ -1830,7 +1830,7 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
+      <c r="A23" s="9"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
@@ -1839,7 +1839,7 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
+      <c r="A24" s="9"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
@@ -1848,7 +1848,7 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
+      <c r="A25" s="9"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
@@ -1857,7 +1857,7 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="9"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
@@ -1866,7 +1866,7 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
@@ -1875,7 +1875,7 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+      <c r="A28" s="9"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
@@ -1884,7 +1884,7 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
+      <c r="A29" s="9"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
@@ -1893,7 +1893,7 @@
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
+      <c r="A30" s="9"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -1902,7 +1902,7 @@
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
+      <c r="A31" s="9"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
@@ -1911,7 +1911,7 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
@@ -1920,7 +1920,7 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+      <c r="A33" s="9"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
@@ -1929,7 +1929,7 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+      <c r="A34" s="9"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
@@ -1938,7 +1938,7 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
@@ -1947,7 +1947,7 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="A36" s="9"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
@@ -1956,7 +1956,7 @@
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="A37" s="9"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="5"/>
@@ -1965,7 +1965,7 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="A38" s="9"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
@@ -1974,7 +1974,7 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
@@ -1983,7 +1983,7 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="5"/>
@@ -1993,35 +1993,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A1:A40"/>
     <mergeCell ref="B1:I1"/>
@@ -2033,6 +2004,35 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>